<commit_message>
IED Mode added (including documentation)
</commit_message>
<xml_diff>
--- a/scenars/Scenar01_TankSimEnv.xlsx
+++ b/scenars/Scenar01_TankSimEnv.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/PycharmProjects/ThesisSim/scenars/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79AEC91-ADEB-FC48-8A6E-B821CDD76FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD194AA-FE61-7347-9F5C-C891E2DC4DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="23960" xr2:uid="{3D1C2A5C-29BC-C649-ACA2-352E8153772B}"/>
   </bookViews>
@@ -32,10 +32,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -100,445 +96,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="374">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF404B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -552,7 +114,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF404B"/>
+          <bgColor rgb="FF00EDED"/>
         </patternFill>
       </fill>
     </dxf>
@@ -563,2166 +125,11 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF404B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF404B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF404B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF404B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00EDED"/>
       <color rgb="FFFF404B"/>
     </mruColors>
   </colors>
@@ -3037,7 +444,7 @@
   <dimension ref="A1:BM64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15500,212 +12907,19 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="R30:AE30 AE31 R39:AE39 R48:AE48 R57:AE57 AE40 AE49 AE58">
-    <cfRule type="containsText" dxfId="121" priority="56" operator="containsText" text="S">
-      <formula>NOT(ISERROR(SEARCH("S",R30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="57" operator="containsText" text="F">
-      <formula>NOT(ISERROR(SEARCH("F",R30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="58" operator="containsText" text="R">
-      <formula>NOT(ISERROR(SEARCH("R",R30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="59" operator="containsText" text="W">
-      <formula>NOT(ISERROR(SEARCH("W",R30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P31:AD31 P32 P40:AD40 P49:AD49 P58:AD58">
-    <cfRule type="containsText" dxfId="117" priority="52" operator="containsText" text="S">
-      <formula>NOT(ISERROR(SEARCH("S",P31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="53" operator="containsText" text="F">
-      <formula>NOT(ISERROR(SEARCH("F",P31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="54" operator="containsText" text="R">
-      <formula>NOT(ISERROR(SEARCH("R",P31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="55" operator="containsText" text="W">
-      <formula>NOT(ISERROR(SEARCH("W",P31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q32:AE32 Q33">
-    <cfRule type="containsText" dxfId="113" priority="48" operator="containsText" text="S">
-      <formula>NOT(ISERROR(SEARCH("S",Q32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="49" operator="containsText" text="F">
-      <formula>NOT(ISERROR(SEARCH("F",Q32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="50" operator="containsText" text="R">
-      <formula>NOT(ISERROR(SEARCH("R",Q32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="51" operator="containsText" text="W">
-      <formula>NOT(ISERROR(SEARCH("W",Q32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R33:AE34">
-    <cfRule type="containsText" dxfId="109" priority="44" operator="containsText" text="S">
-      <formula>NOT(ISERROR(SEARCH("S",R33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="45" operator="containsText" text="F">
-      <formula>NOT(ISERROR(SEARCH("F",R33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="46" operator="containsText" text="R">
-      <formula>NOT(ISERROR(SEARCH("R",R33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="47" operator="containsText" text="W">
-      <formula>NOT(ISERROR(SEARCH("W",R33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF35:AS35">
-    <cfRule type="containsText" dxfId="105" priority="40" operator="containsText" text="S">
-      <formula>NOT(ISERROR(SEARCH("S",AF35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="41" operator="containsText" text="F">
-      <formula>NOT(ISERROR(SEARCH("F",AF35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="42" operator="containsText" text="R">
-      <formula>NOT(ISERROR(SEARCH("R",AF35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="43" operator="containsText" text="W">
-      <formula>NOT(ISERROR(SEARCH("W",AF35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF30:AS30 AS31 AF39:AS39 AF48:AS48 AF57:AS57 AS40 AS49 AS58">
-    <cfRule type="containsText" dxfId="101" priority="36" operator="containsText" text="S">
-      <formula>NOT(ISERROR(SEARCH("S",AF30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="37" operator="containsText" text="F">
-      <formula>NOT(ISERROR(SEARCH("F",AF30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="38" operator="containsText" text="R">
-      <formula>NOT(ISERROR(SEARCH("R",AF30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="39" operator="containsText" text="W">
-      <formula>NOT(ISERROR(SEARCH("W",AF30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF31:AR31 AF40:AR40 AF49:AR49 AF58:AR58">
-    <cfRule type="containsText" dxfId="97" priority="32" operator="containsText" text="S">
-      <formula>NOT(ISERROR(SEARCH("S",AF31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="33" operator="containsText" text="F">
-      <formula>NOT(ISERROR(SEARCH("F",AF31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="34" operator="containsText" text="R">
-      <formula>NOT(ISERROR(SEARCH("R",AF31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="35" operator="containsText" text="W">
-      <formula>NOT(ISERROR(SEARCH("W",AF31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF32:AS32">
-    <cfRule type="containsText" dxfId="93" priority="28" operator="containsText" text="S">
-      <formula>NOT(ISERROR(SEARCH("S",AF32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="29" operator="containsText" text="F">
-      <formula>NOT(ISERROR(SEARCH("F",AF32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="30" operator="containsText" text="R">
-      <formula>NOT(ISERROR(SEARCH("R",AF32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="31" operator="containsText" text="W">
-      <formula>NOT(ISERROR(SEARCH("W",AF32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF33:AS34">
-    <cfRule type="containsText" dxfId="89" priority="24" operator="containsText" text="S">
-      <formula>NOT(ISERROR(SEARCH("S",AF33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="25" operator="containsText" text="F">
-      <formula>NOT(ISERROR(SEARCH("F",AF33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="26" operator="containsText" text="R">
-      <formula>NOT(ISERROR(SEARCH("R",AF33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="27" operator="containsText" text="W">
-      <formula>NOT(ISERROR(SEARCH("W",AF33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AT35:BG35">
-    <cfRule type="containsText" dxfId="85" priority="20" operator="containsText" text="S">
-      <formula>NOT(ISERROR(SEARCH("S",AT35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="21" operator="containsText" text="F">
-      <formula>NOT(ISERROR(SEARCH("F",AT35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="22" operator="containsText" text="R">
-      <formula>NOT(ISERROR(SEARCH("R",AT35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="23" operator="containsText" text="W">
-      <formula>NOT(ISERROR(SEARCH("W",AT35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AT30:AU30 BG31 AT39:AU39 AT48:AU48 AT57:AU57 BG40 BG49 BG58">
-    <cfRule type="containsText" dxfId="81" priority="16" operator="containsText" text="S">
-      <formula>NOT(ISERROR(SEARCH("S",AT30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="17" operator="containsText" text="F">
-      <formula>NOT(ISERROR(SEARCH("F",AT30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="18" operator="containsText" text="R">
-      <formula>NOT(ISERROR(SEARCH("R",AT30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="19" operator="containsText" text="W">
-      <formula>NOT(ISERROR(SEARCH("W",AT30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AT31:BF31 AT40:BF40 AT49:BF49 AT58:BF58">
-    <cfRule type="containsText" dxfId="77" priority="12" operator="containsText" text="S">
-      <formula>NOT(ISERROR(SEARCH("S",AT31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="13" operator="containsText" text="F">
-      <formula>NOT(ISERROR(SEARCH("F",AT31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="14" operator="containsText" text="R">
-      <formula>NOT(ISERROR(SEARCH("R",AT31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="15" operator="containsText" text="W">
-      <formula>NOT(ISERROR(SEARCH("W",AT31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AT32:BG32">
-    <cfRule type="containsText" dxfId="73" priority="8" operator="containsText" text="S">
-      <formula>NOT(ISERROR(SEARCH("S",AT32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="9" operator="containsText" text="F">
-      <formula>NOT(ISERROR(SEARCH("F",AT32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="10" operator="containsText" text="R">
-      <formula>NOT(ISERROR(SEARCH("R",AT32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="11" operator="containsText" text="W">
-      <formula>NOT(ISERROR(SEARCH("W",AT32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AT33:BG34">
-    <cfRule type="containsText" dxfId="69" priority="4" operator="containsText" text="S">
-      <formula>NOT(ISERROR(SEARCH("S",AT33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="5" operator="containsText" text="F">
-      <formula>NOT(ISERROR(SEARCH("F",AT33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="6" operator="containsText" text="R">
-      <formula>NOT(ISERROR(SEARCH("R",AT33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="7" operator="containsText" text="W">
-      <formula>NOT(ISERROR(SEARCH("W",AT33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A1:BL64">
-    <cfRule type="cellIs" dxfId="65" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="64" operator="equal">
       <formula>99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="63" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="65" operator="between">
       <formula>9</formula>
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>80</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>